<commit_message>
standardize core methods, get rid of ascii_name, include subarchive in webservice args
</commit_message>
<xml_diff>
--- a/resources/templates/opus.xlsx
+++ b/resources/templates/opus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbrandt/code/alexweb/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbrandt/code/alexweb/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9655FD21-B349-F140-ADDC-F15EEFDBF742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7FEED7-8604-A949-8525-2566AB3B28F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18960" yWindow="20340" windowWidth="37780" windowHeight="17760" xr2:uid="{A4BFC58D-643C-A848-A1EC-4B4155D53582}"/>
   </bookViews>

</xml_diff>

<commit_message>
asynchronous translation, debug option to start flask service, fix opus template, sticky table headers
</commit_message>
<xml_diff>
--- a/resources/templates/opus.xlsx
+++ b/resources/templates/opus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbrandt/code/alexweb/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7FEED7-8604-A949-8525-2566AB3B28F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76D2422-D671-6B4F-B900-62263F6D6C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18960" yWindow="20340" windowWidth="37780" windowHeight="17760" xr2:uid="{A4BFC58D-643C-A848-A1EC-4B4155D53582}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20800" xr2:uid="{A4BFC58D-643C-A848-A1EC-4B4155D53582}"/>
   </bookViews>
   <sheets>
     <sheet name="{shortname}" sheetId="1" r:id="rId1"/>
@@ -113,9 +113,6 @@
     <t>{col[0]:link_status}</t>
   </si>
   <si>
-    <t>{col[3]}</t>
-  </si>
-  <si>
     <t>{col}</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>version:</t>
+  </si>
+  <si>
+    <t>{col[2]}</t>
   </si>
 </sst>
 </file>
@@ -899,7 +899,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -972,7 +972,7 @@
       <c r="N2" s="40"/>
       <c r="O2" s="40"/>
       <c r="P2" s="51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q2" s="40"/>
       <c r="R2" s="40"/>
@@ -1009,7 +1009,7 @@
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
       <c r="P3" s="52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
@@ -1029,7 +1029,7 @@
       <c r="A4" s="29"/>
       <c r="B4" s="28"/>
       <c r="C4" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="35" t="s">
         <v>17</v>
@@ -1064,10 +1064,10 @@
       <c r="A5" s="12"/>
       <c r="B5" s="30"/>
       <c r="C5" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="53" t="s">
         <v>29</v>
-      </c>
-      <c r="D5" s="53" t="s">
-        <v>30</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="33"/>
@@ -1197,40 +1197,40 @@
         <v>19</v>
       </c>
       <c r="C8" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="50" t="s">
-        <v>26</v>
-      </c>
       <c r="E8" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8" s="46" t="s">
         <v>24</v>
       </c>
       <c r="I8" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J8" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K8" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L8" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M8" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N8" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>

</xml_diff>